<commit_message>
added the documentation of MEDIAN and MODE user defined functions
</commit_message>
<xml_diff>
--- a/a.xlsx
+++ b/a.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Year4\2\ProgrammingLanguages\Practical\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Year4\2\ProgrammingLanguages\Practical\NayaZidan_OudishoQattyne_AgathyHomsy_ShahdAlallaf_Y4_C5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87B9D71-58AF-4947-B766-A07F02FB5AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FAD868A-67C8-49B8-ACA7-E4C56BF58C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BD2884FD-2237-4720-B0E3-16A90B5EC174}"/>
   </bookViews>
@@ -374,13 +374,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AAD7478-A56A-4662-A161-96412E0D77EB}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -412,7 +414,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="B5">
         <v>5</v>

</xml_diff>